<commit_message>
temp class added for bulk PC orders creation
</commit_message>
<xml_diff>
--- a/src/test/resources/ordersECC/ordersECC.xlsx
+++ b/src/test/resources/ordersECC/ordersECC.xlsx
@@ -2,41 +2,133 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
-  <workbookPr/>
-  <mc:AlternateContent>
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Eclipse_Workspace\RF-Automation\qa-automation\src\test\resources\ordersECC\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15240" windowHeight="1455"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="ConsultantOrders" r:id="rId1" sheetId="1"/>
+    <sheet name="ConsultantAdhocOrder" r:id="rId1" sheetId="1"/>
+    <sheet name="PCAdhocOrder" r:id="rId2" sheetId="2"/>
+    <sheet name="RCAdhocOrder" r:id="rId3" sheetId="3"/>
   </sheets>
-  <calcPr calcId="0" iterate="1" iterateDelta="1E-4"/>
+  <calcPr calcId="162913"/>
+  <extLst>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
-  <si>
-    <t>555</t>
-  </si>
-  <si>
-    <t>666</t>
-  </si>
-  <si>
-    <t>444</t>
-  </si>
-  <si>
-    <t>0006234764</t>
-  </si>
-  <si>
-    <t>0006234770</t>
-  </si>
-  <si>
-    <t>0006234772</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+  <si>
+    <t>00881</t>
+  </si>
+  <si>
+    <t>00882</t>
+  </si>
+  <si>
+    <t>00883</t>
+  </si>
+  <si>
+    <t>00884</t>
+  </si>
+  <si>
+    <t>00885</t>
+  </si>
+  <si>
+    <t>00661</t>
+  </si>
+  <si>
+    <t>00662</t>
+  </si>
+  <si>
+    <t>00663</t>
+  </si>
+  <si>
+    <t>00664</t>
+  </si>
+  <si>
+    <t>00665</t>
+  </si>
+  <si>
+    <t>00441</t>
+  </si>
+  <si>
+    <t>00442</t>
+  </si>
+  <si>
+    <t>00443</t>
+  </si>
+  <si>
+    <t>00444</t>
+  </si>
+  <si>
+    <t>00445</t>
+  </si>
+  <si>
+    <t>OrderNumbers</t>
+  </si>
+  <si>
+    <t>008181</t>
+  </si>
+  <si>
+    <t>008182</t>
+  </si>
+  <si>
+    <t>008183</t>
+  </si>
+  <si>
+    <t>008184</t>
+  </si>
+  <si>
+    <t>008185</t>
+  </si>
+  <si>
+    <t>006161</t>
+  </si>
+  <si>
+    <t>006162</t>
+  </si>
+  <si>
+    <t>006163</t>
+  </si>
+  <si>
+    <t>006164</t>
+  </si>
+  <si>
+    <t>006165</t>
+  </si>
+  <si>
+    <t>004141</t>
+  </si>
+  <si>
+    <t>004142</t>
+  </si>
+  <si>
+    <t>004143</t>
+  </si>
+  <si>
+    <t>004144</t>
+  </si>
+  <si>
+    <t>004145</t>
+  </si>
+  <si>
+    <t>0006235673</t>
+  </si>
+  <si>
+    <t>0006235676</t>
+  </si>
+  <si>
+    <t>0006235680</t>
+  </si>
+  <si>
+    <t>0006235682</t>
+  </si>
+  <si>
+    <t>0006235685</t>
   </si>
 </sst>
 </file>
@@ -46,10 +138,11 @@
   <numFmts count="0"/>
   <fonts count="1">
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -70,14 +163,10 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -141,9 +230,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -176,9 +265,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -364,9 +453,55 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+    </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
orders scripts for ECC integration
</commit_message>
<xml_diff>
--- a/src/test/resources/ordersECC/ordersECC.xlsx
+++ b/src/test/resources/ordersECC/ordersECC.xlsx
@@ -4,16 +4,18 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13530" windowHeight="4275" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="ConsultantAdhocOrder" r:id="rId1" sheetId="1"/>
-    <sheet name="PCAdhocOrder" r:id="rId2" sheetId="2"/>
-    <sheet name="RCAdhocOrder" r:id="rId3" sheetId="3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
+    <sheet name="ConsultantAdhocOrder_US" sheetId="5" r:id="rId2"/>
+    <sheet name="PCAdhocOrder_US" sheetId="6" r:id="rId3"/>
+    <sheet name="RCAdhocOrder_US" sheetId="7" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:L12"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -21,122 +23,52 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
-  <si>
-    <t>00881</t>
-  </si>
-  <si>
-    <t>00882</t>
-  </si>
-  <si>
-    <t>00883</t>
-  </si>
-  <si>
-    <t>00884</t>
-  </si>
-  <si>
-    <t>00885</t>
-  </si>
-  <si>
-    <t>00661</t>
-  </si>
-  <si>
-    <t>00662</t>
-  </si>
-  <si>
-    <t>00663</t>
-  </si>
-  <si>
-    <t>00664</t>
-  </si>
-  <si>
-    <t>00665</t>
-  </si>
-  <si>
-    <t>00441</t>
-  </si>
-  <si>
-    <t>00442</t>
-  </si>
-  <si>
-    <t>00443</t>
-  </si>
-  <si>
-    <t>00444</t>
-  </si>
-  <si>
-    <t>00445</t>
-  </si>
-  <si>
-    <t>OrderNumbers</t>
-  </si>
-  <si>
-    <t>008181</t>
-  </si>
-  <si>
-    <t>008182</t>
-  </si>
-  <si>
-    <t>008183</t>
-  </si>
-  <si>
-    <t>008184</t>
-  </si>
-  <si>
-    <t>008185</t>
-  </si>
-  <si>
-    <t>006161</t>
-  </si>
-  <si>
-    <t>006162</t>
-  </si>
-  <si>
-    <t>006163</t>
-  </si>
-  <si>
-    <t>006164</t>
-  </si>
-  <si>
-    <t>006165</t>
-  </si>
-  <si>
-    <t>004141</t>
-  </si>
-  <si>
-    <t>004142</t>
-  </si>
-  <si>
-    <t>004143</t>
-  </si>
-  <si>
-    <t>004144</t>
-  </si>
-  <si>
-    <t>004145</t>
-  </si>
-  <si>
-    <t>0006235673</t>
-  </si>
-  <si>
-    <t>0006235676</t>
-  </si>
-  <si>
-    <t>0006235680</t>
-  </si>
-  <si>
-    <t>0006235682</t>
-  </si>
-  <si>
-    <t>0006235685</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
+  <si>
+    <t>0006239503</t>
+  </si>
+  <si>
+    <t>REDEFINE ACUTE CARE REDEFINE Special</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Visa</t>
+  </si>
+  <si>
+    <t>Mar 6, 2017 3:55 AM</t>
+  </si>
+  <si>
+    <t>280.91</t>
+  </si>
+  <si>
+    <t>text.account.order.status.display.</t>
+  </si>
+  <si>
+    <t>0006239505</t>
+  </si>
+  <si>
+    <t>Mar 6, 2017 3:59 AM</t>
+  </si>
+  <si>
+    <t>327.87</t>
+  </si>
+  <si>
+    <t>0006239511</t>
+  </si>
+  <si>
+    <t>Mar 6, 2017 4:04 AM</t>
+  </si>
+  <si>
+    <t>364.91</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -446,65 +378,127 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="true"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>33</v>
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>35</v>
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated the scripts for ECC orders
</commit_message>
<xml_diff>
--- a/src/test/resources/ordersECC/ordersECC.xlsx
+++ b/src/test/resources/ordersECC/ordersECC.xlsx
@@ -1,69 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
-  <workbookPr filterPrivacy="1"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13530" windowHeight="4275" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
-    <sheet name="ConsultantAdhocOrder_US" sheetId="5" r:id="rId2"/>
-    <sheet name="PCAdhocOrder_US" sheetId="6" r:id="rId3"/>
-    <sheet name="RCAdhocOrder_US" sheetId="7" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1:L12"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
-  <si>
-    <t>0006239503</t>
-  </si>
-  <si>
-    <t>REDEFINE ACUTE CARE REDEFINE Special</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>Visa</t>
-  </si>
-  <si>
-    <t>Mar 6, 2017 3:55 AM</t>
-  </si>
-  <si>
-    <t>280.91</t>
-  </si>
-  <si>
-    <t>text.account.order.status.display.</t>
-  </si>
-  <si>
-    <t>0006239505</t>
-  </si>
-  <si>
-    <t>Mar 6, 2017 3:59 AM</t>
-  </si>
-  <si>
-    <t>327.87</t>
-  </si>
-  <si>
-    <t>0006239511</t>
-  </si>
-  <si>
-    <t>Mar 6, 2017 4:04 AM</t>
-  </si>
-  <si>
-    <t>364.91</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -381,124 +333,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
billing shipping  class updated
</commit_message>
<xml_diff>
--- a/src/test/resources/ordersECC/ordersECC.xlsx
+++ b/src/test/resources/ordersECC/ordersECC.xlsx
@@ -8,19 +8,139 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ConsultantAdhocOrder_US" r:id="rId5" sheetId="2"/>
+    <sheet name="PCAdhocOrder_US" r:id="rId6" sheetId="3"/>
+    <sheet name="RCAdhocOrder_US" r:id="rId7" sheetId="4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="37">
+  <si>
+    <t>USER_EMAIL</t>
+  </si>
+  <si>
+    <t>ORDER_NUMBER</t>
+  </si>
+  <si>
+    <t>PRODUCT_NAME</t>
+  </si>
+  <si>
+    <t>ITEM_QTY</t>
+  </si>
+  <si>
+    <t>CARD_TYPE</t>
+  </si>
+  <si>
+    <t>ORDER_DATE</t>
+  </si>
+  <si>
+    <t>TOTAL_PRICE</t>
+  </si>
+  <si>
+    <t>ORDER_STATUS</t>
+  </si>
+  <si>
+    <t>autoconswpwcrp20170315185754@mailinator.com</t>
+  </si>
+  <si>
+    <t>0006260762</t>
+  </si>
+  <si>
+    <t>UNBLEMISH Regimen for Acne</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Visa</t>
+  </si>
+  <si>
+    <t>Mar 16, 2017 3:32 AM</t>
+  </si>
+  <si>
+    <t>177.99</t>
+  </si>
+  <si>
+    <t>Submitted</t>
+  </si>
+  <si>
+    <t>0006260769</t>
+  </si>
+  <si>
+    <t>MasterCard</t>
+  </si>
+  <si>
+    <t>Mar 16, 2017 3:37 AM</t>
+  </si>
+  <si>
+    <t>text.account.order.status.display.</t>
+  </si>
+  <si>
+    <t>0006260774</t>
+  </si>
+  <si>
+    <t>Discover</t>
+  </si>
+  <si>
+    <t>Mar 16, 2017 3:41 AM</t>
+  </si>
+  <si>
+    <t>autopcwpwsspon20170315144640@mailinator.com</t>
+  </si>
+  <si>
+    <t>0006260788</t>
+  </si>
+  <si>
+    <t>Mar 16, 2017 3:49 AM</t>
+  </si>
+  <si>
+    <t>486.00</t>
+  </si>
+  <si>
+    <t>0006260793</t>
+  </si>
+  <si>
+    <t>Mar 16, 2017 3:54 AM</t>
+  </si>
+  <si>
+    <t>162.00</t>
+  </si>
+  <si>
+    <t>autorc20170315134951@mailinator.com</t>
+  </si>
+  <si>
+    <t>0006260798</t>
+  </si>
+  <si>
+    <t>Mar 16, 2017 3:58 AM</t>
+  </si>
+  <si>
+    <t>1,093.03</t>
+  </si>
+  <si>
+    <t>0006260811</t>
+  </si>
+  <si>
+    <t>Mar 16, 2017 4:06 AM</t>
+  </si>
+  <si>
+    <t>373.03</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -339,4 +459,303 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>